<commit_message>
Added Verification & Validation Evidence.
</commit_message>
<xml_diff>
--- a/Documentation/Verification&ValidationEvidence.xlsx
+++ b/Documentation/Verification&ValidationEvidence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjhog\Documents\Personal\Projects\SparcChallenge\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9F7912C-FDD1-47CF-AAD8-4B8D9511E800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF7667D-C753-4B07-82C7-2A8215306F6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3990" yWindow="2790" windowWidth="28800" windowHeight="15435" xr2:uid="{33FFD227-50BA-4B91-A19D-A12E18D0034F}"/>
+    <workbookView xWindow="8565" yWindow="5565" windowWidth="28800" windowHeight="15435" xr2:uid="{33FFD227-50BA-4B91-A19D-A12E18D0034F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,9 +35,71 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+  <si>
+    <t>UR</t>
+  </si>
+  <si>
+    <t>Figure 1:</t>
+  </si>
+  <si>
+    <t>Remote method of loading profile is SMS (as shown in figure 1).</t>
+  </si>
+  <si>
+    <t>Profile loading is initiated via SMS (as shown in figure 1).</t>
+  </si>
+  <si>
+    <t>The pilot's profile specifications are returned upon successful confirmation of authorization.</t>
+  </si>
+  <si>
+    <t>Figure 2:</t>
+  </si>
+  <si>
+    <t>Pilot is checked for authorization and notified of failure (as shown in figure X).</t>
+  </si>
+  <si>
+    <t>Unauthorized pilots cannot receive confirmation of profile loading, as the profile is never loaded (per UR-55)</t>
+  </si>
+  <si>
+    <t>Pilot initiates authorization and profile loading via SMS and receives a confirmation/rejection/failure message regarding the status of the profile loading process via SMS. No other interface is allowed for or described.</t>
+  </si>
+  <si>
+    <t>See compliance for UR-70.</t>
+  </si>
+  <si>
+    <t>In the case that profile loading cannot be completed, a failure message is sent to the pilot via SMS (as shown in figure 2).</t>
+  </si>
+  <si>
+    <t>The specified program has no capability to write to the External Drive.</t>
+  </si>
+  <si>
+    <t>Figure 4:</t>
+  </si>
+  <si>
+    <t>The supplied system and all supporting files currently consume 12 MB of storage (shown in figure 4). There is no concern of reaching 2 GB of storage.</t>
+  </si>
+  <si>
+    <t>The app was built using the .NET 6.0 framework and compiled to a .exe file and is thus perfectly compatible with both Windows 10 and 11. Additionally, the program consumed a maximum observed value of around 60 MB of memory (leaving plenty of memory unallocated) and a hardly observable amount of CPU power (as shown in figure 5).</t>
+  </si>
+  <si>
+    <t>Figure 5:</t>
+  </si>
+  <si>
+    <t>Figure 3:</t>
+  </si>
+  <si>
+    <t>All observed SMS notifications from the system (Confirmation, rejection, and unavailability messages) were received in fewer than 4 seconds from the completion of the sending of the initial SMS message from the pilot's phone.</t>
+  </si>
+  <si>
+    <t>Compliance</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,13 +107,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -66,8 +140,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -83,6 +162,187 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>28576</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>21060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>518382</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91007766-7C4F-CE1F-1A4A-4C7D76CC996F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11144251" y="783060"/>
+          <a:ext cx="1709006" cy="3588915"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>32372</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>237697</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>75629</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{798D21FC-0DF5-D0D8-31DE-4DC6048481BD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11148047" y="4972049"/>
+          <a:ext cx="2034125" cy="2714055"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>41276</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>527504</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DAA150A-EAE2-B5F2-FE4A-8B7F763573AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12985751" y="781051"/>
+          <a:ext cx="1705428" cy="3581399"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>267801</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8187C6BE-6842-1C96-7367-7C7499F9BBB1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13554075" y="5514975"/>
+          <a:ext cx="2096601" cy="2667000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,14 +642,182 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08D3A711-43D0-441B-A3BA-51BF2DC99689}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="82.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>40</v>
+      </c>
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>45</v>
+      </c>
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>50</v>
+      </c>
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>55</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>60</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>70</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>80</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>100</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>110</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>120</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>130</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>140</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>150</v>
+      </c>
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>160</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>170</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K20" t="s">
+        <v>12</v>
+      </c>
+      <c r="O20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>